<commit_message>
testing fix for issue on windows vm
</commit_message>
<xml_diff>
--- a/preprocessor/benchmark_results/windows/omp_threads_only/matrix_mult/2021_06_03--06_42__windows__matrix_mult__runs_20__.xlsx
+++ b/preprocessor/benchmark_results/windows/omp_threads_only/matrix_mult/2021_06_03--06_42__windows__matrix_mult__runs_20__.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" mc:Ignorable="x15 xr xr6 xr10">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Caleb\PycharmProjects\OpenMPy\preprocessor\benchmark_results\windows\omp_threads_only\matrix_mult\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/calebhuck/PycharmProjects/OpenMPy/preprocessor/benchmark_results/windows/omp_threads_only/matrix_mult/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{F3B66C06-4A4E-4590-A782-7DBFC189C510}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067E1C04-DC12-2940-9CDE-171D61A2D2B5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="37220" windowHeight="21820"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="37220" windowHeight="21820" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="2021_06_03--06_42__windows__mat" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="18" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5731,16 +5731,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>0</xdr:col>
-      <xdr:colOff>593725</xdr:colOff>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>12701</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>288925</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5768,15 +5768,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>9</xdr:col>
-      <xdr:colOff>22225</xdr:colOff>
+      <xdr:colOff>12701</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>6350</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>327025</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>33</xdr:row>
-      <xdr:rowOff>171450</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -5804,15 +5804,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>17</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
+      <xdr:colOff>12700</xdr:colOff>
       <xdr:row>19</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>12700</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>12700</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -6136,16 +6136,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AA18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A14" sqref="A14:AA18"/>
+      <selection activeCell="I39" sqref="I39"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B1">
         <v>10</v>
       </c>
@@ -6225,7 +6225,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -6308,7 +6308,7 @@
         <v>30.053100037574701</v>
       </c>
     </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -6391,7 +6391,7 @@
         <v>16.0467499971389</v>
       </c>
     </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>4</v>
       </c>
@@ -6474,7 +6474,7 @@
         <v>9.9046500086784306</v>
       </c>
     </row>
-    <row r="5" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>8</v>
       </c>
@@ -6557,7 +6557,7 @@
         <v>6.5741500139236404</v>
       </c>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A6">
         <v>12</v>
       </c>
@@ -6640,7 +6640,7 @@
         <v>5.5820000290870597</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B8">
         <v>10</v>
       </c>
@@ -6720,7 +6720,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A9">
         <v>2</v>
       </c>
@@ -6803,7 +6803,7 @@
         <v>1.8728465292307099</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A10">
         <v>4</v>
       </c>
@@ -6886,7 +6886,7 @@
         <v>3.0342414937673001</v>
       </c>
     </row>
-    <row r="11" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A11">
         <v>8</v>
       </c>
@@ -6969,7 +6969,7 @@
         <v>4.57140466431769</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A12">
         <v>12</v>
       </c>
@@ -7052,7 +7052,7 @@
         <v>5.3839304695399504</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:27" x14ac:dyDescent="0.2">
       <c r="B14">
         <v>10</v>
       </c>
@@ -7132,7 +7132,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A15">
         <v>2</v>
       </c>
@@ -7215,7 +7215,7 @@
         <v>0.93642326461535896</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A16">
         <v>4</v>
       </c>
@@ -7298,7 +7298,7 @@
         <v>0.75856037344182503</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A17">
         <v>8</v>
       </c>
@@ -7381,7 +7381,7 @@
         <v>0.57142558303971103</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.2">
       <c r="A18">
         <v>12</v>
       </c>

</xml_diff>